<commit_message>
completed cheatsheet for JS H2
</commit_message>
<xml_diff>
--- a/cheatsheetJS.xlsx
+++ b/cheatsheetJS.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="151">
   <si>
     <t>Taalcomponenten</t>
   </si>
@@ -423,6 +423,60 @@
   </si>
   <si>
     <t>Een string is een stuk tekst en geef je aan tussen aanhalingstekens</t>
+  </si>
+  <si>
+    <t>onchange</t>
+  </si>
+  <si>
+    <t>onblur</t>
+  </si>
+  <si>
+    <t>onfocus</t>
+  </si>
+  <si>
+    <t>onselect</t>
+  </si>
+  <si>
+    <t>onsubmit</t>
+  </si>
+  <si>
+    <t>onreset</t>
+  </si>
+  <si>
+    <t>Een element is gewijzigd</t>
+  </si>
+  <si>
+    <t>Een element raakt buiten focus</t>
+  </si>
+  <si>
+    <t>Een element heeft de focus</t>
+  </si>
+  <si>
+    <t>Een element is geselecteerd</t>
+  </si>
+  <si>
+    <t>Het formulier is gereset</t>
+  </si>
+  <si>
+    <t>Het formulier is verstuurd</t>
+  </si>
+  <si>
+    <t>onkeydown</t>
+  </si>
+  <si>
+    <t>Een toets wordt ingedrukt</t>
+  </si>
+  <si>
+    <t>onkeypress</t>
+  </si>
+  <si>
+    <t>Een toets wordt ingedrukt en losgelaten</t>
+  </si>
+  <si>
+    <t>onkeyup</t>
+  </si>
+  <si>
+    <t>Een toets wordt losgelaten</t>
   </si>
 </sst>
 </file>
@@ -465,7 +519,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -525,28 +579,54 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color theme="1" tint="4.9989318521683403E-2"/>
+      </left>
+      <right style="thick">
+        <color theme="1" tint="4.9989318521683403E-2"/>
+      </right>
+      <top style="thick">
+        <color theme="1" tint="4.9989318521683403E-2"/>
+      </top>
+      <bottom style="thick">
+        <color theme="1" tint="4.9989318521683403E-2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color theme="1" tint="4.9989318521683403E-2"/>
+      </left>
+      <right style="thick">
+        <color theme="1" tint="4.9989318521683403E-2"/>
+      </right>
+      <top style="thick">
+        <color theme="1" tint="4.9989318521683403E-2"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -555,8 +635,14 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -567,9 +653,24 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -884,39 +985,41 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9EE6D0E-E614-4978-ACC6-BC1D800059AD}">
-  <dimension ref="A1:I73"/>
+  <dimension ref="A1:I82"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+      <selection activeCell="H86" sqref="H86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" customWidth="1"/>
-    <col min="2" max="2" width="10.42578125" customWidth="1"/>
-    <col min="4" max="4" width="9.28515625" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="13" customWidth="1"/>
+    <col min="2" max="2" width="10.42578125" style="13" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" style="13"/>
+    <col min="4" max="4" width="9.28515625" style="13" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="13"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="5" t="s">
+      <c r="B1" s="10"/>
+      <c r="C1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
+      <c r="I1" s="10"/>
     </row>
     <row r="2" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="2"/>
+      <c r="B2" s="4"/>
       <c r="C2" s="4" t="s">
         <v>8</v>
       </c>
@@ -928,10 +1031,10 @@
       <c r="I2" s="4"/>
     </row>
     <row r="3" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="2"/>
+      <c r="B3" s="4"/>
       <c r="C3" s="4" t="s">
         <v>9</v>
       </c>
@@ -943,10 +1046,10 @@
       <c r="I3" s="4"/>
     </row>
     <row r="4" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="2"/>
+      <c r="B4" s="4"/>
       <c r="C4" s="4" t="s">
         <v>10</v>
       </c>
@@ -958,8 +1061,8 @@
       <c r="I4" s="4"/>
     </row>
     <row r="5" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
+      <c r="A5" s="4"/>
+      <c r="B5" s="4"/>
       <c r="C5" s="4" t="s">
         <v>12</v>
       </c>
@@ -971,10 +1074,10 @@
       <c r="I5" s="4"/>
     </row>
     <row r="6" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="2"/>
+      <c r="B6" s="4"/>
       <c r="C6" s="4" t="s">
         <v>13</v>
       </c>
@@ -986,10 +1089,10 @@
       <c r="I6" s="4"/>
     </row>
     <row r="7" spans="1:9" ht="21" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="2"/>
+      <c r="B7" s="4"/>
       <c r="C7" s="4" t="s">
         <v>132</v>
       </c>
@@ -1001,10 +1104,10 @@
       <c r="I7" s="4"/>
     </row>
     <row r="8" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="2"/>
+      <c r="B8" s="4"/>
       <c r="C8" s="4" t="s">
         <v>14</v>
       </c>
@@ -1017,188 +1120,188 @@
     </row>
     <row r="9" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="10" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="6"/>
-      <c r="B10" s="7" t="s">
+      <c r="A10" s="2"/>
+      <c r="B10" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="C10" s="7"/>
-      <c r="D10" s="10" t="s">
+      <c r="C10" s="5"/>
+      <c r="D10" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="E10" s="11"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="12"/>
-      <c r="H10" s="7" t="s">
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="9"/>
+      <c r="H10" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="I10" s="7"/>
+      <c r="I10" s="5"/>
     </row>
     <row r="11" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="3" t="s">
+      <c r="A11" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2" t="s">
+      <c r="C11" s="4"/>
+      <c r="D11" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2">
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="4">
         <v>15</v>
       </c>
-      <c r="I11" s="2"/>
+      <c r="I11" s="4"/>
     </row>
     <row r="12" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="3" t="s">
+      <c r="A12" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2" t="s">
+      <c r="C12" s="4"/>
+      <c r="D12" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
-      <c r="H12" s="2">
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="4">
         <v>14</v>
       </c>
-      <c r="I12" s="2"/>
+      <c r="I12" s="4"/>
     </row>
     <row r="13" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="8" t="s">
+      <c r="A13" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2" t="s">
+      <c r="C13" s="4"/>
+      <c r="D13" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
-      <c r="H13" s="2">
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="4"/>
+      <c r="H13" s="4">
         <v>15</v>
       </c>
-      <c r="I13" s="2"/>
+      <c r="I13" s="4"/>
     </row>
     <row r="14" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="8" t="s">
+      <c r="A14" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2" t="s">
+      <c r="C14" s="4"/>
+      <c r="D14" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
-      <c r="H14" s="2">
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="4"/>
+      <c r="H14" s="4">
         <v>14</v>
       </c>
-      <c r="I14" s="2"/>
+      <c r="I14" s="4"/>
     </row>
     <row r="15" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="3" t="s">
+      <c r="A15" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B15" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2" t="s">
+      <c r="C15" s="4"/>
+      <c r="D15" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
-      <c r="G15" s="2"/>
-      <c r="H15" s="2">
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="4"/>
+      <c r="H15" s="4">
         <v>24</v>
       </c>
-      <c r="I15" s="2"/>
+      <c r="I15" s="4"/>
     </row>
     <row r="16" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="3" t="s">
+      <c r="A16" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B16" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2" t="s">
+      <c r="C16" s="4"/>
+      <c r="D16" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2"/>
-      <c r="H16" s="2">
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="4"/>
+      <c r="H16" s="4">
         <v>14</v>
       </c>
-      <c r="I16" s="2"/>
+      <c r="I16" s="4"/>
     </row>
     <row r="17" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="3" t="s">
+      <c r="A17" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B17" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2" t="s">
+      <c r="C17" s="4"/>
+      <c r="D17" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
-      <c r="G17" s="2"/>
-      <c r="H17" s="2">
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="4"/>
+      <c r="H17" s="4">
         <v>28</v>
       </c>
-      <c r="I17" s="2"/>
+      <c r="I17" s="4"/>
     </row>
     <row r="18" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="3" t="s">
+      <c r="A18" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B18" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2" t="s">
+      <c r="C18" s="4"/>
+      <c r="D18" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
-      <c r="G18" s="2"/>
-      <c r="H18" s="2">
+      <c r="E18" s="4"/>
+      <c r="F18" s="4"/>
+      <c r="G18" s="4"/>
+      <c r="H18" s="4">
         <v>14</v>
       </c>
-      <c r="I18" s="2"/>
+      <c r="I18" s="4"/>
     </row>
     <row r="19" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="20" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="9" t="s">
+      <c r="A20" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="B20" s="9"/>
-      <c r="C20" s="9"/>
-      <c r="D20" s="9" t="s">
+      <c r="B20" s="5"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="E20" s="9"/>
-      <c r="F20" s="9"/>
-      <c r="G20" s="9"/>
-      <c r="H20" s="9"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="5"/>
+      <c r="G20" s="5"/>
+      <c r="H20" s="5"/>
     </row>
     <row r="21" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="4" t="s">
@@ -1440,203 +1543,203 @@
     </row>
     <row r="38" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="39" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="7" t="s">
+      <c r="A39" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="B39" s="7"/>
-      <c r="C39" s="7" t="s">
+      <c r="B39" s="5"/>
+      <c r="C39" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="D39" s="7"/>
-      <c r="E39" s="7"/>
-      <c r="F39" s="7" t="s">
+      <c r="D39" s="5"/>
+      <c r="E39" s="5"/>
+      <c r="F39" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="G39" s="7"/>
-      <c r="H39" s="7"/>
-      <c r="I39" s="7"/>
+      <c r="G39" s="5"/>
+      <c r="H39" s="5"/>
+      <c r="I39" s="5"/>
     </row>
     <row r="40" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="13" t="s">
+      <c r="A40" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="B40" s="2"/>
-      <c r="C40" s="2" t="s">
+      <c r="B40" s="4"/>
+      <c r="C40" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="D40" s="2"/>
-      <c r="E40" s="2"/>
-      <c r="F40" s="2" t="s">
+      <c r="D40" s="4"/>
+      <c r="E40" s="4"/>
+      <c r="F40" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="G40" s="2"/>
-      <c r="H40" s="2"/>
-      <c r="I40" s="2"/>
+      <c r="G40" s="4"/>
+      <c r="H40" s="4"/>
+      <c r="I40" s="4"/>
     </row>
     <row r="41" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="13" t="s">
+      <c r="A41" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="B41" s="2"/>
-      <c r="C41" s="2" t="s">
+      <c r="B41" s="4"/>
+      <c r="C41" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="D41" s="2"/>
-      <c r="E41" s="2"/>
-      <c r="F41" s="2" t="s">
+      <c r="D41" s="4"/>
+      <c r="E41" s="4"/>
+      <c r="F41" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="G41" s="2"/>
-      <c r="H41" s="2"/>
-      <c r="I41" s="2"/>
+      <c r="G41" s="4"/>
+      <c r="H41" s="4"/>
+      <c r="I41" s="4"/>
     </row>
     <row r="42" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="2" t="s">
+      <c r="A42" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="B42" s="2"/>
-      <c r="C42" s="2" t="s">
+      <c r="B42" s="4"/>
+      <c r="C42" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="D42" s="2"/>
-      <c r="E42" s="2"/>
-      <c r="F42" s="2" t="s">
+      <c r="D42" s="4"/>
+      <c r="E42" s="4"/>
+      <c r="F42" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="G42" s="2"/>
-      <c r="H42" s="2"/>
-      <c r="I42" s="2"/>
+      <c r="G42" s="4"/>
+      <c r="H42" s="4"/>
+      <c r="I42" s="4"/>
     </row>
     <row r="43" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="2" t="s">
+      <c r="A43" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="B43" s="2"/>
-      <c r="C43" s="2" t="s">
+      <c r="B43" s="4"/>
+      <c r="C43" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="D43" s="2"/>
-      <c r="E43" s="2"/>
-      <c r="F43" s="2" t="s">
+      <c r="D43" s="4"/>
+      <c r="E43" s="4"/>
+      <c r="F43" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="G43" s="2"/>
-      <c r="H43" s="2"/>
-      <c r="I43" s="2"/>
+      <c r="G43" s="4"/>
+      <c r="H43" s="4"/>
+      <c r="I43" s="4"/>
     </row>
     <row r="44" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="2" t="s">
+      <c r="A44" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="B44" s="2"/>
-      <c r="C44" s="2" t="s">
+      <c r="B44" s="4"/>
+      <c r="C44" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="D44" s="2"/>
-      <c r="E44" s="2"/>
-      <c r="F44" s="2" t="s">
+      <c r="D44" s="4"/>
+      <c r="E44" s="4"/>
+      <c r="F44" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="G44" s="2"/>
-      <c r="H44" s="2"/>
-      <c r="I44" s="2"/>
+      <c r="G44" s="4"/>
+      <c r="H44" s="4"/>
+      <c r="I44" s="4"/>
     </row>
     <row r="45" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="2" t="s">
+      <c r="A45" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="B45" s="2"/>
-      <c r="C45" s="2" t="s">
+      <c r="B45" s="4"/>
+      <c r="C45" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="D45" s="2"/>
-      <c r="E45" s="2"/>
-      <c r="F45" s="2" t="s">
+      <c r="D45" s="4"/>
+      <c r="E45" s="4"/>
+      <c r="F45" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="G45" s="2"/>
-      <c r="H45" s="2"/>
-      <c r="I45" s="2"/>
+      <c r="G45" s="4"/>
+      <c r="H45" s="4"/>
+      <c r="I45" s="4"/>
     </row>
     <row r="46" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="2" t="s">
+      <c r="A46" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="B46" s="2"/>
-      <c r="C46" s="2" t="s">
+      <c r="B46" s="4"/>
+      <c r="C46" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="D46" s="2"/>
-      <c r="E46" s="2"/>
-      <c r="F46" s="2" t="s">
+      <c r="D46" s="4"/>
+      <c r="E46" s="4"/>
+      <c r="F46" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="G46" s="2"/>
-      <c r="H46" s="2"/>
-      <c r="I46" s="2"/>
+      <c r="G46" s="4"/>
+      <c r="H46" s="4"/>
+      <c r="I46" s="4"/>
     </row>
     <row r="47" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="2" t="s">
+      <c r="A47" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="B47" s="2"/>
-      <c r="C47" s="2" t="s">
+      <c r="B47" s="4"/>
+      <c r="C47" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="D47" s="2"/>
-      <c r="E47" s="2"/>
-      <c r="F47" s="2" t="s">
+      <c r="D47" s="4"/>
+      <c r="E47" s="4"/>
+      <c r="F47" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="G47" s="2"/>
-      <c r="H47" s="2"/>
-      <c r="I47" s="2"/>
+      <c r="G47" s="4"/>
+      <c r="H47" s="4"/>
+      <c r="I47" s="4"/>
     </row>
     <row r="48" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="2" t="s">
+      <c r="A48" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="B48" s="2"/>
-      <c r="C48" s="2" t="s">
+      <c r="B48" s="4"/>
+      <c r="C48" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="D48" s="2"/>
-      <c r="E48" s="2"/>
-      <c r="F48" s="2" t="s">
+      <c r="D48" s="4"/>
+      <c r="E48" s="4"/>
+      <c r="F48" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="G48" s="2"/>
-      <c r="H48" s="2"/>
-      <c r="I48" s="2"/>
+      <c r="G48" s="4"/>
+      <c r="H48" s="4"/>
+      <c r="I48" s="4"/>
     </row>
     <row r="49" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="2" t="s">
+      <c r="A49" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="B49" s="2"/>
-      <c r="C49" s="2" t="s">
+      <c r="B49" s="4"/>
+      <c r="C49" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="D49" s="2"/>
-      <c r="E49" s="2"/>
-      <c r="F49" s="2" t="s">
+      <c r="D49" s="4"/>
+      <c r="E49" s="4"/>
+      <c r="F49" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="G49" s="2"/>
-      <c r="H49" s="2"/>
-      <c r="I49" s="2"/>
+      <c r="G49" s="4"/>
+      <c r="H49" s="4"/>
+      <c r="I49" s="4"/>
     </row>
     <row r="50" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="51" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="52" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="9" t="s">
+      <c r="A52" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="B52" s="9"/>
-      <c r="C52" s="9"/>
-      <c r="D52" s="9"/>
-      <c r="E52" s="9"/>
-      <c r="F52" s="9"/>
+      <c r="B52" s="5"/>
+      <c r="C52" s="5"/>
+      <c r="D52" s="5"/>
+      <c r="E52" s="5"/>
+      <c r="F52" s="5"/>
     </row>
     <row r="53" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="4" t="s">
@@ -1700,14 +1803,14 @@
     </row>
     <row r="58" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="59" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="9" t="s">
+      <c r="A59" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="B59" s="9"/>
-      <c r="C59" s="9"/>
-      <c r="D59" s="9"/>
-      <c r="E59" s="9"/>
-      <c r="F59" s="9"/>
+      <c r="B59" s="5"/>
+      <c r="C59" s="5"/>
+      <c r="D59" s="5"/>
+      <c r="E59" s="5"/>
+      <c r="F59" s="5"/>
     </row>
     <row r="60" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A60" s="4" t="s">
@@ -1769,208 +1872,291 @@
       </c>
       <c r="F64" s="4"/>
     </row>
-    <row r="65" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="66" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A66" s="7" t="s">
+    <row r="65" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="66" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A66" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="B66" s="7"/>
-      <c r="C66" s="7"/>
-      <c r="D66" s="7" t="s">
+      <c r="B66" s="5"/>
+      <c r="C66" s="5"/>
+      <c r="D66" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="E66" s="7"/>
-      <c r="F66" s="7"/>
-      <c r="G66" s="7"/>
-      <c r="H66" s="7"/>
-    </row>
-    <row r="67" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A67" s="2" t="s">
+      <c r="E66" s="5"/>
+      <c r="F66" s="5"/>
+      <c r="G66" s="5"/>
+      <c r="H66" s="5"/>
+    </row>
+    <row r="67" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A67" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="B67" s="2"/>
-      <c r="C67" s="2"/>
-      <c r="D67" s="2" t="s">
+      <c r="B67" s="4"/>
+      <c r="C67" s="4"/>
+      <c r="D67" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="E67" s="2"/>
-      <c r="F67" s="2"/>
-      <c r="G67" s="2"/>
-      <c r="H67" s="2"/>
-    </row>
-    <row r="68" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A68" s="2" t="s">
+      <c r="E67" s="4"/>
+      <c r="F67" s="4"/>
+      <c r="G67" s="4"/>
+      <c r="H67" s="4"/>
+    </row>
+    <row r="68" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A68" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="B68" s="2"/>
-      <c r="C68" s="2"/>
-      <c r="D68" s="2" t="s">
+      <c r="B68" s="4"/>
+      <c r="C68" s="4"/>
+      <c r="D68" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="E68" s="2"/>
-      <c r="F68" s="2"/>
-      <c r="G68" s="2"/>
-      <c r="H68" s="2"/>
-    </row>
-    <row r="69" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A69" s="2" t="s">
+      <c r="E68" s="4"/>
+      <c r="F68" s="4"/>
+      <c r="G68" s="4"/>
+      <c r="H68" s="4"/>
+    </row>
+    <row r="69" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A69" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="B69" s="2"/>
-      <c r="C69" s="2"/>
-      <c r="D69" s="2" t="s">
+      <c r="B69" s="4"/>
+      <c r="C69" s="4"/>
+      <c r="D69" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="E69" s="2"/>
-      <c r="F69" s="2"/>
-      <c r="G69" s="2"/>
-      <c r="H69" s="2"/>
-    </row>
-    <row r="70" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A70" s="2" t="s">
+      <c r="E69" s="4"/>
+      <c r="F69" s="4"/>
+      <c r="G69" s="4"/>
+      <c r="H69" s="4"/>
+    </row>
+    <row r="70" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A70" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="B70" s="2"/>
-      <c r="C70" s="2"/>
-      <c r="D70" s="2" t="s">
+      <c r="B70" s="4"/>
+      <c r="C70" s="4"/>
+      <c r="D70" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="E70" s="2"/>
-      <c r="F70" s="2"/>
-      <c r="G70" s="2"/>
-      <c r="H70" s="2"/>
-    </row>
-    <row r="71" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A71" s="2" t="s">
+      <c r="E70" s="4"/>
+      <c r="F70" s="4"/>
+      <c r="G70" s="4"/>
+      <c r="H70" s="4"/>
+    </row>
+    <row r="71" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A71" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="B71" s="2"/>
-      <c r="C71" s="2"/>
-      <c r="D71" s="2" t="s">
+      <c r="B71" s="4"/>
+      <c r="C71" s="4"/>
+      <c r="D71" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="E71" s="2"/>
-      <c r="F71" s="2"/>
-      <c r="G71" s="2"/>
-      <c r="H71" s="2"/>
-    </row>
-    <row r="72" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A72" s="2" t="s">
+      <c r="E71" s="4"/>
+      <c r="F71" s="4"/>
+      <c r="G71" s="4"/>
+      <c r="H71" s="4"/>
+    </row>
+    <row r="72" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A72" s="11" t="s">
         <v>102</v>
       </c>
-      <c r="B72" s="2"/>
-      <c r="C72" s="2"/>
-      <c r="D72" s="2" t="s">
+      <c r="B72" s="11"/>
+      <c r="C72" s="11"/>
+      <c r="D72" s="11" t="s">
         <v>103</v>
       </c>
-      <c r="E72" s="2"/>
-      <c r="F72" s="2"/>
-      <c r="G72" s="2"/>
-      <c r="H72" s="2"/>
-    </row>
-    <row r="73" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+      <c r="E72" s="11"/>
+      <c r="F72" s="11"/>
+      <c r="G72" s="11"/>
+      <c r="H72" s="11"/>
+    </row>
+    <row r="73" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A73" s="12" t="s">
+        <v>133</v>
+      </c>
+      <c r="B73" s="12"/>
+      <c r="C73" s="12"/>
+      <c r="D73" s="12" t="s">
+        <v>139</v>
+      </c>
+      <c r="E73" s="12"/>
+      <c r="F73" s="12"/>
+      <c r="G73" s="12"/>
+      <c r="H73" s="12"/>
+    </row>
+    <row r="74" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A74" s="12" t="s">
+        <v>134</v>
+      </c>
+      <c r="B74" s="12"/>
+      <c r="C74" s="12"/>
+      <c r="D74" s="12" t="s">
+        <v>140</v>
+      </c>
+      <c r="E74" s="12"/>
+      <c r="F74" s="12"/>
+      <c r="G74" s="12"/>
+      <c r="H74" s="12"/>
+    </row>
+    <row r="75" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A75" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="B75" s="12"/>
+      <c r="C75" s="12"/>
+      <c r="D75" s="12" t="s">
+        <v>141</v>
+      </c>
+      <c r="E75" s="12"/>
+      <c r="F75" s="12"/>
+      <c r="G75" s="12"/>
+      <c r="H75" s="12"/>
+    </row>
+    <row r="76" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A76" s="12" t="s">
+        <v>136</v>
+      </c>
+      <c r="B76" s="12"/>
+      <c r="C76" s="12"/>
+      <c r="D76" s="12" t="s">
+        <v>142</v>
+      </c>
+      <c r="E76" s="12"/>
+      <c r="F76" s="12"/>
+      <c r="G76" s="12"/>
+      <c r="H76" s="12"/>
+    </row>
+    <row r="77" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A77" s="14" t="s">
+        <v>137</v>
+      </c>
+      <c r="B77" s="14"/>
+      <c r="C77" s="14"/>
+      <c r="D77" s="14" t="s">
+        <v>144</v>
+      </c>
+      <c r="E77" s="14"/>
+      <c r="F77" s="14"/>
+      <c r="G77" s="14"/>
+      <c r="H77" s="14"/>
+      <c r="I77" s="15"/>
+    </row>
+    <row r="78" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A78" s="16" t="s">
+        <v>138</v>
+      </c>
+      <c r="B78" s="16"/>
+      <c r="C78" s="16"/>
+      <c r="D78" s="16" t="s">
+        <v>143</v>
+      </c>
+      <c r="E78" s="16"/>
+      <c r="F78" s="16"/>
+      <c r="G78" s="16"/>
+      <c r="H78" s="16"/>
+      <c r="I78" s="15"/>
+    </row>
+    <row r="79" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A79" s="17" t="s">
+        <v>145</v>
+      </c>
+      <c r="B79" s="18"/>
+      <c r="C79" s="19"/>
+      <c r="D79" s="17" t="s">
+        <v>146</v>
+      </c>
+      <c r="E79" s="18"/>
+      <c r="F79" s="18"/>
+      <c r="G79" s="18"/>
+      <c r="H79" s="19"/>
+      <c r="I79" s="15"/>
+    </row>
+    <row r="80" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A80" s="17" t="s">
+        <v>147</v>
+      </c>
+      <c r="B80" s="18"/>
+      <c r="C80" s="19"/>
+      <c r="D80" s="17" t="s">
+        <v>148</v>
+      </c>
+      <c r="E80" s="18"/>
+      <c r="F80" s="18"/>
+      <c r="G80" s="18"/>
+      <c r="H80" s="19"/>
+      <c r="I80" s="15"/>
+    </row>
+    <row r="81" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A81" s="17" t="s">
+        <v>149</v>
+      </c>
+      <c r="B81" s="18"/>
+      <c r="C81" s="19"/>
+      <c r="D81" s="17" t="s">
+        <v>150</v>
+      </c>
+      <c r="E81" s="18"/>
+      <c r="F81" s="18"/>
+      <c r="G81" s="18"/>
+      <c r="H81" s="19"/>
+      <c r="I81" s="15"/>
+    </row>
+    <row r="82" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A82" s="15"/>
+      <c r="B82" s="15"/>
+      <c r="C82" s="15"/>
+      <c r="D82" s="15"/>
+      <c r="E82" s="15"/>
+      <c r="F82" s="15"/>
+      <c r="G82" s="15"/>
+      <c r="H82" s="15"/>
+      <c r="I82" s="15"/>
+    </row>
   </sheetData>
-  <mergeCells count="148">
-    <mergeCell ref="D72:H72"/>
-    <mergeCell ref="D71:H71"/>
-    <mergeCell ref="D69:H69"/>
-    <mergeCell ref="D70:H70"/>
-    <mergeCell ref="D68:H68"/>
-    <mergeCell ref="A60:D60"/>
-    <mergeCell ref="D67:H67"/>
-    <mergeCell ref="D66:H66"/>
-    <mergeCell ref="A67:C67"/>
-    <mergeCell ref="A66:C66"/>
-    <mergeCell ref="A72:C72"/>
-    <mergeCell ref="A71:C71"/>
-    <mergeCell ref="A70:C70"/>
-    <mergeCell ref="A69:C69"/>
-    <mergeCell ref="A68:C68"/>
-    <mergeCell ref="A59:F59"/>
-    <mergeCell ref="E64:F64"/>
-    <mergeCell ref="E63:F63"/>
-    <mergeCell ref="E62:F62"/>
-    <mergeCell ref="E61:F61"/>
-    <mergeCell ref="E60:F60"/>
-    <mergeCell ref="A64:D64"/>
-    <mergeCell ref="A63:D63"/>
-    <mergeCell ref="A62:D62"/>
-    <mergeCell ref="A61:D61"/>
-    <mergeCell ref="E57:F57"/>
-    <mergeCell ref="A57:D57"/>
-    <mergeCell ref="A56:D56"/>
-    <mergeCell ref="A55:D55"/>
-    <mergeCell ref="A54:D54"/>
-    <mergeCell ref="A53:D53"/>
-    <mergeCell ref="A52:F52"/>
-    <mergeCell ref="E56:F56"/>
-    <mergeCell ref="E55:F55"/>
-    <mergeCell ref="E54:F54"/>
-    <mergeCell ref="E53:F53"/>
-    <mergeCell ref="F44:I44"/>
-    <mergeCell ref="F43:I43"/>
-    <mergeCell ref="F42:I42"/>
-    <mergeCell ref="F41:I41"/>
-    <mergeCell ref="F40:I40"/>
-    <mergeCell ref="F39:I39"/>
-    <mergeCell ref="C49:E49"/>
-    <mergeCell ref="F49:I49"/>
-    <mergeCell ref="F48:I48"/>
-    <mergeCell ref="F47:I47"/>
-    <mergeCell ref="F46:I46"/>
-    <mergeCell ref="F45:I45"/>
-    <mergeCell ref="C39:E39"/>
-    <mergeCell ref="C40:E40"/>
-    <mergeCell ref="C41:E41"/>
-    <mergeCell ref="C42:E42"/>
-    <mergeCell ref="C43:E43"/>
-    <mergeCell ref="C44:E44"/>
-    <mergeCell ref="C45:E45"/>
-    <mergeCell ref="C46:E46"/>
-    <mergeCell ref="C47:E47"/>
-    <mergeCell ref="C48:E48"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="A41:B41"/>
-    <mergeCell ref="A40:B40"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="A49:B49"/>
-    <mergeCell ref="A48:B48"/>
-    <mergeCell ref="A47:B47"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="A44:B44"/>
-    <mergeCell ref="D37:H37"/>
-    <mergeCell ref="D36:H36"/>
-    <mergeCell ref="D35:H35"/>
-    <mergeCell ref="A37:C37"/>
-    <mergeCell ref="A36:C36"/>
-    <mergeCell ref="A35:C35"/>
-    <mergeCell ref="A34:C34"/>
-    <mergeCell ref="A33:C33"/>
-    <mergeCell ref="A32:C32"/>
-    <mergeCell ref="A31:C31"/>
-    <mergeCell ref="A30:C30"/>
-    <mergeCell ref="A29:C29"/>
-    <mergeCell ref="D20:H20"/>
-    <mergeCell ref="D34:H34"/>
-    <mergeCell ref="D33:H33"/>
-    <mergeCell ref="D32:H32"/>
-    <mergeCell ref="D31:H31"/>
-    <mergeCell ref="D30:H30"/>
-    <mergeCell ref="D29:H29"/>
-    <mergeCell ref="D28:H28"/>
-    <mergeCell ref="D27:H27"/>
-    <mergeCell ref="D26:H26"/>
-    <mergeCell ref="D25:H25"/>
-    <mergeCell ref="D24:H24"/>
-    <mergeCell ref="D23:H23"/>
-    <mergeCell ref="D22:H22"/>
-    <mergeCell ref="D21:H21"/>
-    <mergeCell ref="A23:C23"/>
-    <mergeCell ref="A22:C22"/>
-    <mergeCell ref="A21:C21"/>
-    <mergeCell ref="A28:C28"/>
+  <mergeCells count="166">
+    <mergeCell ref="D73:H73"/>
+    <mergeCell ref="A73:C73"/>
+    <mergeCell ref="D81:H81"/>
+    <mergeCell ref="D80:H80"/>
+    <mergeCell ref="D79:H79"/>
+    <mergeCell ref="A81:C81"/>
+    <mergeCell ref="A80:C80"/>
+    <mergeCell ref="A79:C79"/>
+    <mergeCell ref="D77:H77"/>
+    <mergeCell ref="D78:H78"/>
+    <mergeCell ref="A78:C78"/>
+    <mergeCell ref="A77:C77"/>
+    <mergeCell ref="A76:C76"/>
+    <mergeCell ref="D76:H76"/>
+    <mergeCell ref="D75:H75"/>
+    <mergeCell ref="A75:C75"/>
+    <mergeCell ref="A74:C74"/>
+    <mergeCell ref="D74:H74"/>
+    <mergeCell ref="C1:I1"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="C8:I8"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="C7:I7"/>
+    <mergeCell ref="C4:I4"/>
+    <mergeCell ref="C5:I5"/>
+    <mergeCell ref="C6:I6"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="C3:I3"/>
+    <mergeCell ref="C2:I2"/>
     <mergeCell ref="H12:I12"/>
     <mergeCell ref="H11:I11"/>
     <mergeCell ref="H10:I10"/>
@@ -1995,30 +2181,106 @@
     <mergeCell ref="D16:G16"/>
     <mergeCell ref="D15:G15"/>
     <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="C3:I3"/>
-    <mergeCell ref="C2:I2"/>
-    <mergeCell ref="C1:I1"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="C8:I8"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="C7:I7"/>
-    <mergeCell ref="C4:I4"/>
-    <mergeCell ref="C5:I5"/>
-    <mergeCell ref="C6:I6"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A31:C31"/>
+    <mergeCell ref="A30:C30"/>
+    <mergeCell ref="A29:C29"/>
+    <mergeCell ref="D20:H20"/>
+    <mergeCell ref="D34:H34"/>
+    <mergeCell ref="D33:H33"/>
+    <mergeCell ref="D32:H32"/>
+    <mergeCell ref="D31:H31"/>
+    <mergeCell ref="D30:H30"/>
+    <mergeCell ref="D29:H29"/>
+    <mergeCell ref="D28:H28"/>
+    <mergeCell ref="D27:H27"/>
+    <mergeCell ref="D26:H26"/>
+    <mergeCell ref="D25:H25"/>
+    <mergeCell ref="D24:H24"/>
+    <mergeCell ref="D23:H23"/>
+    <mergeCell ref="D22:H22"/>
+    <mergeCell ref="D21:H21"/>
+    <mergeCell ref="A23:C23"/>
+    <mergeCell ref="A22:C22"/>
+    <mergeCell ref="A21:C21"/>
+    <mergeCell ref="A28:C28"/>
+    <mergeCell ref="D37:H37"/>
+    <mergeCell ref="D36:H36"/>
+    <mergeCell ref="D35:H35"/>
+    <mergeCell ref="A37:C37"/>
+    <mergeCell ref="A36:C36"/>
+    <mergeCell ref="A35:C35"/>
+    <mergeCell ref="A34:C34"/>
+    <mergeCell ref="A33:C33"/>
+    <mergeCell ref="A32:C32"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="A41:B41"/>
+    <mergeCell ref="A40:B40"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="A49:B49"/>
+    <mergeCell ref="A48:B48"/>
+    <mergeCell ref="A47:B47"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="A44:B44"/>
+    <mergeCell ref="F44:I44"/>
+    <mergeCell ref="F43:I43"/>
+    <mergeCell ref="F42:I42"/>
+    <mergeCell ref="F41:I41"/>
+    <mergeCell ref="F40:I40"/>
+    <mergeCell ref="F39:I39"/>
+    <mergeCell ref="C49:E49"/>
+    <mergeCell ref="F49:I49"/>
+    <mergeCell ref="F48:I48"/>
+    <mergeCell ref="F47:I47"/>
+    <mergeCell ref="F46:I46"/>
+    <mergeCell ref="F45:I45"/>
+    <mergeCell ref="C39:E39"/>
+    <mergeCell ref="C40:E40"/>
+    <mergeCell ref="C41:E41"/>
+    <mergeCell ref="C42:E42"/>
+    <mergeCell ref="C43:E43"/>
+    <mergeCell ref="C44:E44"/>
+    <mergeCell ref="C45:E45"/>
+    <mergeCell ref="C46:E46"/>
+    <mergeCell ref="C47:E47"/>
+    <mergeCell ref="C48:E48"/>
+    <mergeCell ref="E57:F57"/>
+    <mergeCell ref="A57:D57"/>
+    <mergeCell ref="A56:D56"/>
+    <mergeCell ref="A55:D55"/>
+    <mergeCell ref="A54:D54"/>
+    <mergeCell ref="A53:D53"/>
+    <mergeCell ref="A52:F52"/>
+    <mergeCell ref="E56:F56"/>
+    <mergeCell ref="E55:F55"/>
+    <mergeCell ref="E54:F54"/>
+    <mergeCell ref="E53:F53"/>
+    <mergeCell ref="A59:F59"/>
+    <mergeCell ref="E64:F64"/>
+    <mergeCell ref="E63:F63"/>
+    <mergeCell ref="E62:F62"/>
+    <mergeCell ref="E61:F61"/>
+    <mergeCell ref="E60:F60"/>
+    <mergeCell ref="A64:D64"/>
+    <mergeCell ref="A63:D63"/>
+    <mergeCell ref="A62:D62"/>
+    <mergeCell ref="A61:D61"/>
+    <mergeCell ref="D72:H72"/>
+    <mergeCell ref="D71:H71"/>
+    <mergeCell ref="D69:H69"/>
+    <mergeCell ref="D70:H70"/>
+    <mergeCell ref="D68:H68"/>
+    <mergeCell ref="A60:D60"/>
+    <mergeCell ref="D67:H67"/>
+    <mergeCell ref="D66:H66"/>
+    <mergeCell ref="A67:C67"/>
+    <mergeCell ref="A66:C66"/>
+    <mergeCell ref="A72:C72"/>
+    <mergeCell ref="A71:C71"/>
+    <mergeCell ref="A70:C70"/>
+    <mergeCell ref="A69:C69"/>
+    <mergeCell ref="A68:C68"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>

</xml_diff>